<commit_message>
Thay đổi ràng buộc csdl
</commit_message>
<xml_diff>
--- a/SQLSERVER/SANPHAM.xlsx
+++ b/SQLSERVER/SANPHAM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Van Nghia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Van Nghia\OneDrive\Desktop\DoAn_Winform\DOAN_MonHoc\SQLSERVER\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1381,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
@@ -3557,7 +3557,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" ht="158.4" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>4</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" ht="144" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>16</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" ht="144" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>20</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="144" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>24</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>242</v>
       </c>

</xml_diff>